<commit_message>
cambio opcion rapida link por botones y reinicio legalizador
</commit_message>
<xml_diff>
--- a/src/legalizador/legalizador.xlsx
+++ b/src/legalizador/legalizador.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Olimpostudio\Temporales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\TeamComunicaciones\programa listo\src\legalizador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95715743-F541-49B8-84D4-D6ED415F63EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB5967C-D8D7-4CBF-929D-0C6455BC7B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>idvendedor</t>
   </si>
@@ -53,6 +53,57 @@
   </si>
   <si>
     <t>Mensaje</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 602511579633</t>
+  </si>
+  <si>
+    <t>869466060182485</t>
+  </si>
+  <si>
+    <t>OQUENDO</t>
+  </si>
+  <si>
+    <t>ALEJANDRO</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 602306826399</t>
+  </si>
+  <si>
+    <t>868651052191260</t>
+  </si>
+  <si>
+    <t>CATAÑO</t>
+  </si>
+  <si>
+    <t>ANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 602202936480</t>
+  </si>
+  <si>
+    <t>868651052190171</t>
+  </si>
+  <si>
+    <t>MUÑOZ</t>
+  </si>
+  <si>
+    <t>ANDRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 602308742078</t>
+  </si>
+  <si>
+    <t>355689861577154</t>
+  </si>
+  <si>
+    <t>OLARTE</t>
+  </si>
+  <si>
+    <t>BLANCA</t>
   </si>
 </sst>
 </file>
@@ -108,11 +159,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,22 +470,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -456,6 +515,110 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1010014821</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>3224114582</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>1007524653</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1010014821</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>3102587311</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>43655411</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1010014821</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>3102585958</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>1007524753</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1010014821</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>3124372604</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>65680215</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>